<commit_message>
fixes, crawling on search engine is broken still
</commit_message>
<xml_diff>
--- a/resources/sample.xlsx
+++ b/resources/sample.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/826060f01241f503/Skrivbord/repos/SIMS-WebCrawler/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{574A2737-D5DE-48ED-9437-2A13DEAF859E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEB5B346-D248-48D2-BEBA-0B617396E628}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{574A2737-D5DE-48ED-9437-2A13DEAF859E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9611E385-E56E-464B-A222-307B929F9436}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1755" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5610" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$21217</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$21217</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Norm, Typ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Varumärke</t>
   </si>
@@ -54,31 +51,7 @@
     <t>Typbeteckning</t>
   </si>
   <si>
-    <t>Ritningsnummer</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Beteckning</t>
-  </si>
-  <si>
-    <t>Kompletterande Information övrigt</t>
-  </si>
-  <si>
-    <t>Ref annan</t>
-  </si>
-  <si>
-    <t>Historiskt Varumärke</t>
-  </si>
-  <si>
-    <t>Historiskt inköpsreferens</t>
-  </si>
-  <si>
     <t>Enhet</t>
-  </si>
-  <si>
-    <t>Förpackning</t>
   </si>
   <si>
     <t>SSG-notering</t>
@@ -461,15 +434,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,66 +473,34 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2">
+      <c r="H2">
         <v>2920154</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S21217" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S20">
-      <sortCondition ref="A1:A21217"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
@@ -575,15 +519,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010010C434EB1DB2C840905C129DEF3248A8" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="f5c52abd5abaeca892e2707c0ddfba45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c221e18-ef66-4043-995e-c1f019f7264f" xmlns:ns3="21159b93-ab72-4913-ab76-7074a1720729" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfc38c306cf79085c964c09fee6e8774" ns2:_="" ns3:_="">
     <xsd:import namespace="5c221e18-ef66-4043-995e-c1f019f7264f"/>
@@ -772,6 +707,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CD4EA04-07BB-4E14-B9AF-D357DEFDB98D}">
   <ds:schemaRefs>
@@ -784,14 +728,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD0C223-616F-4D61-8257-367346F1D6A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C049F7F-93D6-40F0-960C-E1529FFD4E3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -808,4 +744,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD0C223-616F-4D61-8257-367346F1D6A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated to carls newest scraper
</commit_message>
<xml_diff>
--- a/resources/sample.xlsx
+++ b/resources/sample.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/826060f01241f503/Skrivbord/repos/SIMS-WebCrawler/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{574A2737-D5DE-48ED-9437-2A13DEAF859E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEB5B346-D248-48D2-BEBA-0B617396E628}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{574A2737-D5DE-48ED-9437-2A13DEAF859E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9611E385-E56E-464B-A222-307B929F9436}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1755" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5610" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$21217</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$21217</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Norm, Typ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Varumärke</t>
   </si>
@@ -54,31 +51,7 @@
     <t>Typbeteckning</t>
   </si>
   <si>
-    <t>Ritningsnummer</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Beteckning</t>
-  </si>
-  <si>
-    <t>Kompletterande Information övrigt</t>
-  </si>
-  <si>
-    <t>Ref annan</t>
-  </si>
-  <si>
-    <t>Historiskt Varumärke</t>
-  </si>
-  <si>
-    <t>Historiskt inköpsreferens</t>
-  </si>
-  <si>
     <t>Enhet</t>
-  </si>
-  <si>
-    <t>Förpackning</t>
   </si>
   <si>
     <t>SSG-notering</t>
@@ -461,15 +434,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,66 +473,34 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2">
+      <c r="H2">
         <v>2920154</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S21217" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S20">
-      <sortCondition ref="A1:A21217"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
@@ -575,15 +519,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010010C434EB1DB2C840905C129DEF3248A8" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="f5c52abd5abaeca892e2707c0ddfba45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c221e18-ef66-4043-995e-c1f019f7264f" xmlns:ns3="21159b93-ab72-4913-ab76-7074a1720729" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfc38c306cf79085c964c09fee6e8774" ns2:_="" ns3:_="">
     <xsd:import namespace="5c221e18-ef66-4043-995e-c1f019f7264f"/>
@@ -772,6 +707,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CD4EA04-07BB-4E14-B9AF-D357DEFDB98D}">
   <ds:schemaRefs>
@@ -784,14 +728,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD0C223-616F-4D61-8257-367346F1D6A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C049F7F-93D6-40F0-960C-E1529FFD4E3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -808,4 +744,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD0C223-616F-4D61-8257-367346F1D6A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>